<commit_message>
avances generarentidades y primer entidad creada automaticamente y funcional (M4sllLitSeguimie)
</commit_message>
<xml_diff>
--- a/generarentidades/generarComandoPython.xlsx
+++ b/generarentidades/generarComandoPython.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\generarentidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD4D08F-E516-4BAB-B58D-209BB9778B47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200D090-3733-4528-9AAD-22122EBB169A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{6B583061-8CCE-48C2-A899-3291AA3A1814}"/>
   </bookViews>
   <sheets>
     <sheet name="generador" sheetId="1" r:id="rId1"/>
     <sheet name="SQL" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Datatypes" sheetId="3" r:id="rId4"/>
+    <sheet name="Datatypes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="208">
-  <si>
-    <t>m4sll_pedido_det</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="213">
   <si>
     <t>secuencia?</t>
   </si>
@@ -39,6 +35,9 @@
     <t>m4sll_doc_litigios</t>
   </si>
   <si>
+    <t>m4sll_lit_seguimie</t>
+  </si>
+  <si>
     <t>nombretablaNEW</t>
   </si>
   <si>
@@ -48,24 +47,21 @@
     <t>Comando</t>
   </si>
   <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>m4sll_litigios</t>
   </si>
   <si>
+    <t>lit_id_litigio,id_organization</t>
+  </si>
+  <si>
+    <t>Templates</t>
+  </si>
+  <si>
     <t>Generar comando</t>
   </si>
   <si>
     <t>lit_id_litigio, id_organization,dol_secuencia</t>
   </si>
   <si>
-    <t>Templates asociados a cierta cantidad de columnas y si cuenta con una secuencia entre las pks</t>
-  </si>
-  <si>
-    <t>Template tabla</t>
-  </si>
-  <si>
     <t>select tab.table_schema,</t>
   </si>
   <si>
@@ -652,13 +648,31 @@
   </si>
   <si>
     <t>String,String,Long</t>
+  </si>
+  <si>
+    <t>sec1</t>
+  </si>
+  <si>
+    <t>sec0</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>https://software.fujitsu.com/jp/manual/manualfiles/m150000/j2ul1738/08enz200/j1738-00-02-04-01.html</t>
+  </si>
+  <si>
+    <t>String,String</t>
+  </si>
+  <si>
+    <t>id_organization,lit_id_litigio,lis_secuencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +714,14 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -753,12 +775,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -771,9 +794,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1087,135 +1112,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C95634-6815-48B1-861A-4160D7F81E45}">
-  <dimension ref="C3:J13"/>
+  <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="111.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="112" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="100" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="B3" s="5"/>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="2" t="str">
-        <f>C10</f>
+      <c r="F4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>A4</f>
         <v>secuencia?</v>
       </c>
-      <c r="G4" s="3" t="str">
-        <f>D10</f>
-        <v>index</v>
-      </c>
       <c r="H4" s="3" t="str">
-        <f>E10</f>
-        <v>Template tabla</v>
+        <f>B4</f>
+        <v>Template</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
-        <v>2</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F5" s="1" t="b">
-        <f>ISNUMBER(SEARCH("secuencia",LOWER(D5)))</f>
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <f t="shared" ref="G5:G7" si="0">IF(COUNTBLANK(F5),"",ISNUMBER(SEARCH("secuencia",LOWER(E5))))</f>
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="b">
-        <f>F5</f>
-        <v>1</v>
-      </c>
       <c r="H5" s="1" t="str">
-        <f>+VLOOKUP(G5,D11:E23,2,FALSE)</f>
-        <v>m4sll_pedido_det</v>
+        <f t="shared" ref="H5:H7" si="1">IF(COUNTBLANK(G5)&gt;0,"",VLOOKUP(G5,A:B,2,FALSE))</f>
+        <v>sec1</v>
       </c>
       <c r="I5" s="6" t="str">
-        <f>LOWER("python generarentidades.py "&amp;C5&amp;" "&amp;SUBSTITUTE(D5," ","")&amp;" "&amp;E5&amp;" "&amp;H5)</f>
-        <v>python generarentidades.py m4sll_doc_litigios lit_id_litigio,id_organization,dol_secuencia string,string,long m4sll_pedido_det</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="b">
-        <f>C11</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="b">
+        <f t="shared" ref="I5:I7" si="2">IF(COUNTBLANK(H5)&gt;0,"","python generarentidades.py "&amp;D5&amp;" "&amp;SUBSTITUTE(LOWER(E5)," ","")&amp;" "&amp;F5&amp;" "&amp;H5)</f>
+        <v>python generarentidades.py m4sll_doc_litigios lit_id_litigio,id_organization,dol_secuencia String,String,Long sec1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="b">
         <f>ISNUMBER(SEARCH("secuencia",#REF!))</f>
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="b">
-        <f t="shared" ref="D12" si="0">C12</f>
+      <c r="B6" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>sec0</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>python generarentidades.py m4sll_litigios lit_id_litigio,id_organization String,String sec0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>sec1</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>python generarentidades.py m4sll_lit_seguimie id_organization,lit_id_litigio,lis_secuencia String,String,Long sec1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="1" t="str">
+        <f>IF(COUNTBLANK(F8),"",ISNUMBER(SEARCH("secuencia",LOWER(E8))))</f>
+        <v/>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f>IF(COUNTBLANK(G8)&gt;0,"",VLOOKUP(G8,A:B,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f>IF(COUNTBLANK(H8)&gt;0,"","python generarentidades.py "&amp;D8&amp;" "&amp;SUBSTITUTE(LOWER(E8)," ","")&amp;" "&amp;F8&amp;" "&amp;H8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1" t="str">
+        <f t="shared" ref="G9:G13" si="3">IF(COUNTBLANK(F9),"",ISNUMBER(SEARCH("secuencia",LOWER(E9))))</f>
+        <v/>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f t="shared" ref="H9:H13" si="4">IF(COUNTBLANK(G9)&gt;0,"",VLOOKUP(G9,A:B,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f t="shared" ref="I9:I13" si="5">IF(COUNTBLANK(H9)&gt;0,"","python generarentidades.py "&amp;D9&amp;" "&amp;SUBSTITUTE(LOWER(E9)," ","")&amp;" "&amp;F9&amp;" "&amp;H9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I10" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I12" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I13" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1226,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED72078-21C9-4990-ABD2-8863B6C157AD}">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1238,567 +1381,567 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1807,25 +1950,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524AA7B6-F59B-4B18-BD97-ED8D0981F2EF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAD7C82-31D3-4F46-B563-BE37F379A951}">
+  <dimension ref="F2:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A55"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAD7C82-31D3-4F46-B563-BE37F379A951}">
-  <dimension ref="F5:H47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="F1:H1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1835,481 +1964,489 @@
     <col min="8" max="8" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F2" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>43</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
         <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>53</v>
-      </c>
-      <c r="H11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>56</v>
-      </c>
-      <c r="H12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
         <v>58</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>59</v>
-      </c>
-      <c r="H13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
         <v>61</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>62</v>
-      </c>
-      <c r="H14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" t="s">
         <v>56</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="s">
         <v>59</v>
-      </c>
-      <c r="H16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
         <v>62</v>
-      </c>
-      <c r="H17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
         <v>67</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>68</v>
-      </c>
-      <c r="H18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
         <v>70</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>71</v>
-      </c>
-      <c r="H19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" t="s">
         <v>73</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>74</v>
-      </c>
-      <c r="H20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" t="s">
         <v>76</v>
-      </c>
-      <c r="G21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H21" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="s">
         <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
         <v>80</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>81</v>
-      </c>
-      <c r="H23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" t="s">
         <v>83</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>84</v>
-      </c>
-      <c r="H24" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" t="s">
         <v>84</v>
-      </c>
-      <c r="H25" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" t="s">
         <v>87</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>88</v>
-      </c>
-      <c r="H26" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" t="s">
         <v>88</v>
-      </c>
-      <c r="H27" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" t="s">
         <v>91</v>
       </c>
-      <c r="G28" t="s">
-        <v>92</v>
-      </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" t="s">
         <v>93</v>
-      </c>
-      <c r="G29" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G30" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" t="s">
         <v>93</v>
-      </c>
-      <c r="H30" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="31" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" t="s">
         <v>96</v>
       </c>
-      <c r="G31" t="s">
-        <v>97</v>
-      </c>
       <c r="H31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" t="s">
         <v>62</v>
-      </c>
-      <c r="H32" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" t="s">
         <v>99</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>100</v>
-      </c>
-      <c r="H33" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" t="s">
         <v>102</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>103</v>
-      </c>
-      <c r="H34" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
+        <v>104</v>
+      </c>
+      <c r="G35" t="s">
         <v>105</v>
       </c>
-      <c r="G35" t="s">
-        <v>106</v>
-      </c>
       <c r="H35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" t="s">
         <v>107</v>
       </c>
-      <c r="G36" t="s">
-        <v>108</v>
-      </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" t="s">
         <v>109</v>
       </c>
-      <c r="G37" t="s">
-        <v>110</v>
-      </c>
       <c r="H37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" t="s">
         <v>111</v>
       </c>
-      <c r="G38" t="s">
-        <v>112</v>
-      </c>
       <c r="H38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" t="s">
         <v>113</v>
       </c>
-      <c r="G39" t="s">
-        <v>114</v>
-      </c>
       <c r="H39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" t="s">
         <v>115</v>
       </c>
-      <c r="G40" t="s">
-        <v>116</v>
-      </c>
       <c r="H40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" t="s">
         <v>117</v>
       </c>
-      <c r="G41" t="s">
-        <v>118</v>
-      </c>
       <c r="H41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F42" t="s">
+        <v>118</v>
+      </c>
+      <c r="G42" t="s">
         <v>119</v>
       </c>
-      <c r="G42" t="s">
-        <v>120</v>
-      </c>
       <c r="H42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{2F68E063-DC62-47C4-A63D-F6A57ABB85BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregado de Astyle.exe para indentacion automatica
</commit_message>
<xml_diff>
--- a/generarentidades/generarComandoPython.xlsx
+++ b/generarentidades/generarComandoPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\generarentidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBFD54B-0DBA-4FB8-9F96-8ED8DA70F153}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A563CF8B-FCEA-4404-BAF7-3C9FD6D9AD31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{6B583061-8CCE-48C2-A899-3291AA3A1814}"/>
   </bookViews>
@@ -50,18 +50,9 @@
     <t>m4sll_litigios</t>
   </si>
   <si>
-    <t>lit_id_litigio,id_organization</t>
-  </si>
-  <si>
-    <t>Templates</t>
-  </si>
-  <si>
     <t>Generar comando</t>
   </si>
   <si>
-    <t>lit_id_litigio, id_organization,dol_secuencia</t>
-  </si>
-  <si>
     <t>select tab.table_schema,</t>
   </si>
   <si>
@@ -672,6 +663,15 @@
   </si>
   <si>
     <t>tpe_id_tp_entidad,id_organization</t>
+  </si>
+  <si>
+    <t>id_organization,lit_id_litigio,dol_secuencia</t>
+  </si>
+  <si>
+    <t>id_organization,lit_id_litigio</t>
+  </si>
+  <si>
+    <t>Lista de Templates</t>
   </si>
 </sst>
 </file>
@@ -1121,15 +1121,16 @@
   <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
@@ -1139,11 +1140,11 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>214</v>
       </c>
       <c r="B3" s="5"/>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1151,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -1160,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G4" s="2" t="str">
         <f>A4</f>
@@ -1178,17 +1179,17 @@
       <c r="A5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>207</v>
+      <c r="B5" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G5" s="1" t="b">
         <f t="shared" ref="G5:G7" si="0">IF(COUNTBLANK(F5),"",ISNUMBER(SEARCH("secuencia",LOWER(E5))))</f>
@@ -1200,7 +1201,7 @@
       </c>
       <c r="I5" s="6" t="str">
         <f t="shared" ref="I5:I7" si="2">IF(COUNTBLANK(H5)&gt;0,"","python generarentidades.py "&amp;D5&amp;" "&amp;SUBSTITUTE(LOWER(E5)," ","")&amp;" "&amp;F5&amp;" "&amp;H5)</f>
-        <v>python generarentidades.py m4sll_doc_litigios lit_id_litigio,id_organization,dol_secuencia String,String,Long sec1</v>
+        <v>python generarentidades.py m4sll_doc_litigios id_organization,lit_id_litigio,dol_secuencia String,String,Long sec1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1208,17 +1209,17 @@
         <f>ISNUMBER(SEARCH("secuencia",#REF!))</f>
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>208</v>
+      <c r="B6" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>7</v>
+        <v>213</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G6" s="1" t="b">
         <f t="shared" si="0"/>
@@ -1230,7 +1231,7 @@
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>python generarentidades.py m4sll_litigios lit_id_litigio,id_organization String,String sec0</v>
+        <v>python generarentidades.py m4sll_litigios id_organization,lit_id_litigio String,String sec0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1238,10 +1239,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G7" s="1" t="b">
         <f t="shared" si="0"/>
@@ -1258,13 +1259,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G8" s="1" t="b">
         <f>IF(COUNTBLANK(F8),"",ISNUMBER(SEARCH("secuencia",LOWER(E8))))</f>
@@ -1393,567 +1394,567 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1978,480 +1979,480 @@
   <sheetData>
     <row r="2" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F2" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F5" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
         <v>73</v>
-      </c>
-      <c r="H21" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F42" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G45" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes mejoras menores generarentidades
</commit_message>
<xml_diff>
--- a/generarentidades/generarComandoPython.xlsx
+++ b/generarentidades/generarComandoPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\generarentidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ED4823-B84B-427B-83EB-FC7EB36CE4F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668A3161-B565-410E-B2EC-A0A42BDF1E2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{6B583061-8CCE-48C2-A899-3291AA3A1814}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="164">
   <si>
     <t>secuencia?</t>
   </si>
@@ -476,168 +476,6 @@
     <t>SELECT * FROM t1;</t>
   </si>
   <si>
-    <t>WITH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   t1 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             SELECT tab.table_schema,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    tab.table_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               FROM information_schema.tables tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              WHERE tab.table_schema NOT IN ('pg_catalog', 'information_schema')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND tab.table_type = 'BASE TABLE'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND tab.table_schema = 'sll'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND tab.table_name = LOWER('m4sll_doc_litigios')</t>
-  </si>
-  <si>
-    <t>), t2 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             SELECT t1.*,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    tco.constraint_name,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    tco.constraint_schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               FROM t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          LEFT JOIN information_schema.table_constraints tco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 ON tco.table_schema = t1.table_schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND tco.table_name = t1.table_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND tco.constraint_type = 'PRIMARY KEY'</t>
-  </si>
-  <si>
-    <t>), t3 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             SELECT t2.*,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    kcu.column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               FROM t2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          LEFT JOIN information_schema.key_column_usage kcu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 ON kcu.constraint_name = t2.constraint_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND kcu.constraint_schema = t2.constraint_schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND kcu.constraint_name = t2.constraint_name</t>
-  </si>
-  <si>
-    <t>), t4 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             SELECT t3.*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  , col.data_type AS sqlserver_data_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               FROM t3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          LEFT JOIN information_schema.columns col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 ON col.column_name = t3.column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND col.table_schema = t3.table_schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                AND col.table_name = t3.table_name</t>
-  </si>
-  <si>
-    <t>), t5 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              SELECT 'bigint'                      AS sqlserver_data_type, 'Long'          AS java_data_type union</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              SELECT 'character varying'           AS sqlserver_data_type, 'String'        AS java_data_type union</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              SELECT 'smallint'                    AS sqlserver_data_type, 'Short'         AS java_data_type union</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              SELECT 'timestamp without time zone' AS sqlserver_data_type, 'java.sql.Time' AS java_data_type</t>
-  </si>
-  <si>
-    <t>), t6 AS (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              SELECT t4.*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                   , t5.java_data_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                FROM t4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           LEFT JOIN t5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  ON t4.sqlserver_data_type = t5.sqlserver_data_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  SELECT table_name,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         string_agg(column_name, ',' ORDER BY column_name DESC) AS key_columns,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         string_agg(java_data_type, ',' ORDER BY column_name DESC) AS key_data_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    FROM t6</t>
-  </si>
-  <si>
-    <t>GROUP BY table_schema,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         table_name,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         constraint_name</t>
-  </si>
-  <si>
-    <t>ORDER BY table_schema,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         table_name</t>
-  </si>
-  <si>
     <t>VIEJOS:</t>
   </si>
   <si>
@@ -672,13 +510,78 @@
   </si>
   <si>
     <t>id_organization,lit_id_litigio</t>
+  </si>
+  <si>
+    <t>schemaNew</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WITH
+   t1 AS (
+             SELECT tab.table_schema,
+                    tab.table_name
+               FROM information_schema.tables tab
+              WHERE tab.table_schema NOT IN ('pg_catalog', 'information_schema')
+                AND tab.table_type = 'BASE TABLE'
+                AND LOWER(tab.table_schema) = ('sll')
+                AND LOWER(tab.table_name) = LOWER('m4sll_doc_litigios')
+), t2 AS (
+             SELECT t1.*,
+                    tco.constraint_name,
+                    tco.constraint_schema
+               FROM t1
+          LEFT JOIN information_schema.table_constraints tco
+                 ON tco.table_schema = t1.table_schema
+                AND tco.table_name = t1.table_name
+                AND tco.constraint_type = 'PRIMARY KEY'
+), t3 AS (
+             SELECT t2.*,
+                    kcu.column_name
+               FROM t2
+          LEFT JOIN information_schema.key_column_usage kcu
+                 ON kcu.constraint_name = t2.constraint_name
+                AND kcu.constraint_schema = t2.constraint_schema
+                AND kcu.constraint_name = t2.constraint_name
+), t4 AS (
+             SELECT t3.*
+                  , col.data_type AS sqlserver_data_type
+               FROM t3
+          LEFT JOIN information_schema.columns col
+                 ON col.column_name = t3.column_name
+                AND col.table_schema = t3.table_schema
+                AND col.table_name = t3.table_name
+), t5 AS (
+              SELECT 'bigint'                      AS sqlserver_data_type, 'Long'          AS java_data_type union
+              SELECT 'character varying'           AS sqlserver_data_type, 'String'        AS java_data_type union
+              SELECT 'smallint'                    AS sqlserver_data_type, 'Short'         AS java_data_type union
+              SELECT 'timestamp without time zone' AS sqlserver_data_type, 'java.sql.Time' AS java_data_type
+), t6 AS (
+              SELECT t4.*
+                   , t5.java_data_type
+                FROM t4
+           LEFT JOIN t5
+                  ON t4.sqlserver_data_type = t5.sqlserver_data_type
+)
+  SELECT table_schema,
+         table_name,
+         string_agg(column_name, ',' ORDER BY column_name DESC) AS key_columns,
+         string_agg(java_data_type, ',' ORDER BY column_name DESC) AS key_data_types
+    FROM t6
+GROUP BY table_schema,
+         table_name,
+         constraint_name
+ORDER BY table_schema,
+         table_name
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +592,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -730,7 +640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,6 +650,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -781,31 +696,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1118,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C95634-6815-48B1-861A-4160D7F81E45}">
-  <dimension ref="A3:J17"/>
+  <dimension ref="A3:K17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1129,245 +1053,266 @@
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="100" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="10" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="H4" s="2" t="str">
         <f>A4</f>
         <v>secuencia?</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="I4" s="3" t="str">
         <f>B4</f>
         <v>Template</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>213</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <f t="shared" ref="G5:G7" si="0">IF(COUNTBLANK(F5),"",ISNUMBER(SEARCH("secuencia",LOWER(E5))))</f>
+        <v>159</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <f t="shared" ref="H5:H7" si="0">IF(COUNTBLANK(G5),"",ISNUMBER(SEARCH("secuencia",LOWER(F5))))</f>
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" ref="H5:H7" si="1">IF(COUNTBLANK(G5)&gt;0,"",VLOOKUP(G5,A:B,2,FALSE))</f>
+      <c r="I5" s="1" t="str">
+        <f t="shared" ref="I5:I7" si="1">IF(COUNTBLANK(H5)&gt;0,"",VLOOKUP(H5,A:B,2,FALSE))</f>
         <v>sec1</v>
       </c>
-      <c r="I5" s="6" t="str">
-        <f t="shared" ref="I5:I7" si="2">IF(COUNTBLANK(H5)&gt;0,"","python generarentidades.py "&amp;D5&amp;" "&amp;SUBSTITUTE(LOWER(E5)," ","")&amp;" "&amp;F5&amp;" "&amp;H5)</f>
-        <v>python generarentidades.py m4sll_doc_litigios id_organization,lit_id_litigio,dol_secuencia String,String,Long sec1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="6" t="str">
+        <f>IF(COUNTBLANK(I5)&gt;0,"","python generarentidades.py "&amp;D5&amp;" "&amp;E5&amp;" "&amp;SUBSTITUTE(LOWER(F5)," ","")&amp;" "&amp;G5&amp;" "&amp;I5)</f>
+        <v>python generarentidades.py sll m4sll_doc_litigios id_organization,lit_id_litigio,dol_secuencia String,String,Long sec1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="b">
         <f>ISNUMBER(SEARCH("secuencia",#REF!))</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" s="1" t="b">
+        <v>160</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="1" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="I6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>sec0</v>
       </c>
-      <c r="I6" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>python generarentidades.py m4sll_litigios id_organization,lit_id_litigio String,String sec0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="6" t="str">
+        <f t="shared" ref="J6:J13" si="2">IF(COUNTBLANK(I6)&gt;0,"","python generarentidades.py "&amp;D6&amp;" "&amp;E6&amp;" "&amp;SUBSTITUTE(LOWER(F6)," ","")&amp;" "&amp;G6&amp;" "&amp;I6)</f>
+        <v>python generarentidades.py sll m4sll_litigios id_organization,lit_id_litigio String,String sec0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>210</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G7" s="1" t="b">
+        <v>156</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="I7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>sec1</v>
       </c>
-      <c r="I7" s="6" t="str">
+      <c r="J7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>python generarentidades.py m4sll_lit_seguimie id_organization,lit_id_litigio,lis_secuencia String,String,Long sec1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>python generarentidades.py sll m4sll_lit_seguimie id_organization,lit_id_litigio,lis_secuencia String,String,Long sec1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <f>IF(COUNTBLANK(F8),"",ISNUMBER(SEARCH("secuencia",LOWER(E8))))</f>
+        <v>158</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <f>IF(COUNTBLANK(G8),"",ISNUMBER(SEARCH("secuencia",LOWER(F8))))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="str">
-        <f>IF(COUNTBLANK(G8)&gt;0,"",VLOOKUP(G8,A:B,2,FALSE))</f>
+      <c r="I8" s="1" t="str">
+        <f>IF(COUNTBLANK(H8)&gt;0,"",VLOOKUP(H8,A:B,2,FALSE))</f>
         <v>sec0</v>
       </c>
-      <c r="I8" s="6" t="str">
-        <f>IF(COUNTBLANK(H8)&gt;0,"","python generarentidades.py "&amp;D8&amp;" "&amp;SUBSTITUTE(LOWER(E8)," ","")&amp;" "&amp;F8&amp;" "&amp;H8)</f>
-        <v>python generarentidades.py m4sll_tp_entidades tpe_id_tp_entidad,id_organization String,String sec0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>python generarentidades.py sll m4sll_tp_entidades tpe_id_tp_entidad,id_organization String,String sec0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="1" t="str">
-        <f t="shared" ref="G9:G13" si="3">IF(COUNTBLANK(F9),"",ISNUMBER(SEARCH("secuencia",LOWER(E9))))</f>
+      <c r="G9" s="4"/>
+      <c r="H9" s="1" t="str">
+        <f t="shared" ref="H9:H13" si="3">IF(COUNTBLANK(G9),"",ISNUMBER(SEARCH("secuencia",LOWER(F9))))</f>
         <v/>
       </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" ref="H9:H13" si="4">IF(COUNTBLANK(G9)&gt;0,"",VLOOKUP(G9,A:B,2,FALSE))</f>
+      <c r="I9" s="1" t="str">
+        <f t="shared" ref="I9:I13" si="4">IF(COUNTBLANK(H9)&gt;0,"",VLOOKUP(H9,A:B,2,FALSE))</f>
         <v/>
       </c>
-      <c r="I9" s="6" t="str">
-        <f t="shared" ref="I9:I13" si="5">IF(COUNTBLANK(H9)&gt;0,"","python generarentidades.py "&amp;D9&amp;" "&amp;SUBSTITUTE(LOWER(E9)," ","")&amp;" "&amp;F9&amp;" "&amp;H9)</f>
+      <c r="J9" s="6" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="1" t="str">
+      <c r="G10" s="4"/>
+      <c r="H10" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="I10" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I10" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="J10" s="6" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="1" t="str">
+      <c r="G11" s="4"/>
+      <c r="H11" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="I11" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I11" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="J11" s="6" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="1" t="str">
+      <c r="G12" s="4"/>
+      <c r="H12" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H12" s="1" t="str">
+      <c r="I12" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I12" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="J12" s="6" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="1" t="str">
+      <c r="G13" s="4"/>
+      <c r="H13" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="I13" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I13" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="J13" s="6" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I17" s="9"/>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1382,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED72078-21C9-4990-ABD2-8863B6C157AD}">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,284 +1337,206 @@
     <col min="2" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="13"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="13"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="13"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="13"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="13"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="13"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="13"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="13"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="13"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="13"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="13"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="12"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1958,6 +1825,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A64"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1967,7 +1837,7 @@
   <dimension ref="F2:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1979,7 +1849,7 @@
   <sheetData>
     <row r="2" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F2" s="10" t="s">
-        <v>208</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajustes query sql en excel
</commit_message>
<xml_diff>
--- a/generarentidades/generarComandoPython.xlsx
+++ b/generarentidades/generarComandoPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\generarentidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668A3161-B565-410E-B2EC-A0A42BDF1E2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA6021B-65B3-4A93-B403-0F63D62AE713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{6B583061-8CCE-48C2-A899-3291AA3A1814}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{6B583061-8CCE-48C2-A899-3291AA3A1814}"/>
   </bookViews>
   <sheets>
     <sheet name="generador" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="217">
   <si>
     <t>secuencia?</t>
   </si>
@@ -476,6 +476,159 @@
     <t>SELECT * FROM t1;</t>
   </si>
   <si>
+    <t>WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   t1 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT tab.table_schema,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    tab.table_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM information_schema.tables tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              WHERE tab.table_schema NOT IN ('pg_catalog', 'information_schema')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND tab.table_type = 'BASE TABLE'</t>
+  </si>
+  <si>
+    <t>), t2 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT t1.*,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    tco.constraint_name,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    tco.constraint_schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM t1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          LEFT JOIN information_schema.table_constraints tco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 ON tco.table_schema = t1.table_schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND tco.table_name = t1.table_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND tco.constraint_type = 'PRIMARY KEY'</t>
+  </si>
+  <si>
+    <t>), t3 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT t2.*,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    kcu.column_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM t2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          LEFT JOIN information_schema.key_column_usage kcu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 ON kcu.constraint_name = t2.constraint_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND kcu.constraint_schema = t2.constraint_schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND kcu.constraint_name = t2.constraint_name</t>
+  </si>
+  <si>
+    <t>), t4 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT t3.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  , col.data_type AS sqlserver_data_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM t3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          LEFT JOIN information_schema.columns col</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 ON col.column_name = t3.column_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND col.table_schema = t3.table_schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND col.table_name = t3.table_name</t>
+  </si>
+  <si>
+    <t>), t5 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              SELECT 'bigint'                      AS sqlserver_data_type, 'Long'          AS java_data_type union</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              SELECT 'character varying'           AS sqlserver_data_type, 'String'        AS java_data_type union</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              SELECT 'smallint'                    AS sqlserver_data_type, 'Short'         AS java_data_type union</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              SELECT 'timestamp without time zone' AS sqlserver_data_type, 'java.sql.Time' AS java_data_type</t>
+  </si>
+  <si>
+    <t>), t6 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              SELECT t4.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   , t5.java_data_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                FROM t4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           LEFT JOIN t5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  ON t4.sqlserver_data_type = t5.sqlserver_data_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         string_agg(column_name, ',' ORDER BY column_name DESC) AS key_columns,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         string_agg(java_data_type, ',' ORDER BY column_name DESC) AS key_data_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FROM t6</t>
+  </si>
+  <si>
+    <t>GROUP BY table_schema,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         table_name,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         constraint_name</t>
+  </si>
+  <si>
+    <t>ORDER BY table_schema,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         table_name</t>
+  </si>
+  <si>
     <t>VIEJOS:</t>
   </si>
   <si>
@@ -518,70 +671,20 @@
     <t>sll</t>
   </si>
   <si>
-    <t xml:space="preserve">WITH
-   t1 AS (
-             SELECT tab.table_schema,
-                    tab.table_name
-               FROM information_schema.tables tab
-              WHERE tab.table_schema NOT IN ('pg_catalog', 'information_schema')
-                AND tab.table_type = 'BASE TABLE'
-                AND LOWER(tab.table_schema) = ('sll')
-                AND LOWER(tab.table_name) = LOWER('m4sll_doc_litigios')
-), t2 AS (
-             SELECT t1.*,
-                    tco.constraint_name,
-                    tco.constraint_schema
-               FROM t1
-          LEFT JOIN information_schema.table_constraints tco
-                 ON tco.table_schema = t1.table_schema
-                AND tco.table_name = t1.table_name
-                AND tco.constraint_type = 'PRIMARY KEY'
-), t3 AS (
-             SELECT t2.*,
-                    kcu.column_name
-               FROM t2
-          LEFT JOIN information_schema.key_column_usage kcu
-                 ON kcu.constraint_name = t2.constraint_name
-                AND kcu.constraint_schema = t2.constraint_schema
-                AND kcu.constraint_name = t2.constraint_name
-), t4 AS (
-             SELECT t3.*
-                  , col.data_type AS sqlserver_data_type
-               FROM t3
-          LEFT JOIN information_schema.columns col
-                 ON col.column_name = t3.column_name
-                AND col.table_schema = t3.table_schema
-                AND col.table_name = t3.table_name
-), t5 AS (
-              SELECT 'bigint'                      AS sqlserver_data_type, 'Long'          AS java_data_type union
-              SELECT 'character varying'           AS sqlserver_data_type, 'String'        AS java_data_type union
-              SELECT 'smallint'                    AS sqlserver_data_type, 'Short'         AS java_data_type union
-              SELECT 'timestamp without time zone' AS sqlserver_data_type, 'java.sql.Time' AS java_data_type
-), t6 AS (
-              SELECT t4.*
-                   , t5.java_data_type
-                FROM t4
-           LEFT JOIN t5
-                  ON t4.sqlserver_data_type = t5.sqlserver_data_type
-)
-  SELECT table_schema,
-         table_name,
-         string_agg(column_name, ',' ORDER BY column_name DESC) AS key_columns,
-         string_agg(java_data_type, ',' ORDER BY column_name DESC) AS key_data_types
-    FROM t6
-GROUP BY table_schema,
-         table_name,
-         constraint_name
-ORDER BY table_schema,
-         table_name
-</t>
+    <t xml:space="preserve">  SELECT table_schema,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               -- AND LOWER(tab.table_schema) = LOWER('sll')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND LOWER(tab.table_name) = LOWER('STD_SUB_GEO_DIV')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,6 +738,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -717,12 +828,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1044,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C95634-6815-48B1-861A-4160D7F81E45}">
   <dimension ref="A3:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,10 +1190,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -1108,19 +1221,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>202</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="H5" s="1" t="b">
         <f t="shared" ref="H5:H7" si="0">IF(COUNTBLANK(G5),"",ISNUMBER(SEARCH("secuencia",LOWER(F5))))</f>
@@ -1141,19 +1254,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="H6" s="1" t="b">
         <f t="shared" si="0"/>
@@ -1170,16 +1283,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="H7" s="1" t="b">
         <f t="shared" si="0"/>
@@ -1196,16 +1309,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="H8" s="1" t="b">
         <f>IF(COUNTBLANK(G8),"",ISNUMBER(SEARCH("secuencia",LOWER(F8))))</f>
@@ -1325,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED72078-21C9-4990-ABD2-8863B6C157AD}">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,263 +1451,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="12" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="12" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="12" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="12" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="12" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="12" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="12" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="12" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="12" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="A28" s="12" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="12" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="12" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="12" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="12" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="12" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="12" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="A35" s="12" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="A36" s="12" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
+      <c r="A37" s="12" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
+      <c r="A38" s="12" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="12" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="12" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="12" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="12" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
+      <c r="A44" s="12" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
+      <c r="A45" s="12" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
+      <c r="A46" s="12" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
+      <c r="A47" s="12" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
+      <c r="A48" s="12" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13"/>
+      <c r="A49" s="12" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
+      <c r="A50" s="12" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
+      <c r="A51" s="12" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
+      <c r="A52" s="12" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13"/>
+      <c r="A53" s="12" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13"/>
+      <c r="A54" s="12" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
+      <c r="A55" s="12" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
+      <c r="A56" s="12" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13"/>
+      <c r="A57" s="12"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13"/>
+      <c r="A58" s="12"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
+      <c r="A59" s="12"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
+      <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13"/>
+      <c r="A61" s="12"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13"/>
+      <c r="A62" s="12"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
+      <c r="A63" s="12"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="12"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="11"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>20</v>
       </c>
@@ -1826,7 +2067,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A64"/>
+    <mergeCell ref="A66:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1849,7 +2090,7 @@
   <sheetData>
     <row r="2" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F2" s="10" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cambios pedidosResource y generarentidades
</commit_message>
<xml_diff>
--- a/generarentidades/generarComandoPython.xlsx
+++ b/generarentidades/generarComandoPython.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\generarentidades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asd\Desktop\laburo\prosegur\proyectos\sll_cloud\sll_cloud\generarentidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA26A9A-3384-47DE-A74F-4BFF353CD302}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93080645-F82C-4C2E-ABDE-71A6D6A61DCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" tabRatio="532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generador" sheetId="1" r:id="rId1"/>
-    <sheet name="SQL" sheetId="2" r:id="rId2"/>
+    <sheet name="SQLTablasMigradas" sheetId="2" r:id="rId2"/>
     <sheet name="ResultadoSQL" sheetId="4" r:id="rId3"/>
     <sheet name="EnElServer" sheetId="6" r:id="rId4"/>
     <sheet name="Datatypes" sheetId="3" r:id="rId5"/>
+    <sheet name="SQLTablasAmigrar" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EnElServer!$A$2:$A$173</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="642">
   <si>
     <t>Templates</t>
   </si>
@@ -1856,13 +1857,115 @@
   </si>
   <si>
     <t>sll_vw_autor_reu</t>
+  </si>
+  <si>
+    <t>-------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>WITH t1 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             -------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             -- Primera selección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM all_tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              WHERE owner = 'M4GLOBAL'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                AND (   table_name LIKE 'M4SLL%'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     OR table_name IN ('STD_GEO_DIV','STD_GEO_PLACE','STD_SUB_GEO_DIV','STD_COUNTRY','STD_LEG_ENT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   , t2 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             -- Detectar de la lista anterior los backups, repetidos, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             SELECT a.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FROM t1 a, t1 b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              WHERE (    a.table_name LIKE '%' || b.table_name || '%'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     AND LENGTH(a.table_name)&gt;LENGTH(b.table_name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     AND (    REGEXP_LIKE(REPLACE(REPLACE( a.table_name, b.table_name, '' ), '_', '' ), '^[[:digit:]]+$') -- la diferencia entre ambos es numerica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          OR  REPLACE( a.table_name, b.table_name, '' ) LIKE '%BK%' -- la diferencia contiene BK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          OR  REPLACE( a.table_name, b.table_name, '' ) LIKE '%PRUEBA%' -- la diferencia contiene PRUEBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          OR  REPLACE( a.table_name, b.table_name, '' ) LIKE '%_QA' -- termina en QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 OR a.table_name LIKE '%_BKP' -- Hay tablas backup que no tienen su original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   , t3 AS (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             -- Restar ambas listas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            SELECT t1.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              FROM t1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             WHERE t1.table_name NOT IN (SELECT t2.table_name FROM t2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      SELECT table_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        FROM t3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ORDER BY table_name;</t>
+  </si>
+  <si>
+    <t>-- Generar una lista de las tablas a migrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          OR  REPLACE( a.table_name, b.table_name, '' ) LIKE '%_VW_%' -- vistas</t>
+  </si>
+  <si>
+    <t>pag_secuencia|Long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1934,6 +2037,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2117,7 +2226,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2158,6 +2267,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Bad" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -2546,9 +2657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U246"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2560,7 +2671,7 @@
     <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.21875" customWidth="1"/>
+    <col min="8" max="8" width="57" customWidth="1"/>
     <col min="9" max="9" width="57.44140625" customWidth="1"/>
     <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="62.109375" customWidth="1"/>
@@ -4124,7 +4235,10 @@
       </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D26" s="8"/>
+      <c r="D26" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G26,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E26">
         <f>IF(COUNTBLANK(G26)&gt;0,"",COUNTIF(G$4:G26,"?*"))</f>
         <v>23</v>
@@ -4189,7 +4303,10 @@
       </c>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D27" s="8"/>
+      <c r="D27" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G27,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E27">
         <f>IF(COUNTBLANK(G27)&gt;0,"",COUNTIF(G$4:G27,"?*"))</f>
         <v>24</v>
@@ -4708,6 +4825,10 @@
       </c>
     </row>
     <row r="35" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D35" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G35,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E35">
         <f>IF(COUNTBLANK(G35)&gt;0,"",COUNTIF(G$4:G35,"?*"))</f>
         <v>31</v>
@@ -4728,7 +4849,7 @@
       <c r="J35" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="26"/>
       <c r="L35" s="17" t="str">
         <f t="shared" si="0"/>
         <v>start /wait python generarentidades.py</v>
@@ -4770,7 +4891,10 @@
       </c>
     </row>
     <row r="36" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D36" s="8"/>
+      <c r="D36" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G36,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E36">
         <f>IF(COUNTBLANK(G36)&gt;0,"",COUNTIF(G$4:G36,"?*"))</f>
         <v>32</v>
@@ -4831,7 +4955,10 @@
       </c>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G37,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E37">
         <f>IF(COUNTBLANK(G37)&gt;0,"",COUNTIF(G$4:G37,"?*"))</f>
         <v>33</v>
@@ -5039,45 +5166,47 @@
         <v>pag_secuencia|Long,lit_id_litigio|String,id_organization|String</v>
       </c>
       <c r="I40" s="26" t="s">
-        <v>526</v>
-      </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="K40" s="10"/>
       <c r="L40" s="17" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>start /wait python generarentidades.py</v>
       </c>
       <c r="M40" s="17" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>sll</v>
       </c>
       <c r="N40" s="17" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>m4sll_pagos</v>
       </c>
       <c r="O40" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>"lit_id_litigio|String,id_organization|String"</v>
       </c>
       <c r="P40" s="17" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>"pag_secuencia|Long"</v>
       </c>
       <c r="Q40" s="17" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="R40" s="17" t="str">
+        <v>""</v>
+      </c>
+      <c r="R40" s="17" t="b">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="S40" s="17" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>sec1</v>
       </c>
       <c r="T40" s="4" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>start /wait python generarentidades.py sll m4sll_pagos "lit_id_litigio|String,id_organization|String" "pag_secuencia|Long" "" sec1</v>
       </c>
       <c r="U40" s="30" t="s">
         <v>526</v>
@@ -5342,6 +5471,10 @@
       </c>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D45" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G45,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v>x</v>
+      </c>
       <c r="E45">
         <f>IF(COUNTBLANK(G45)&gt;0,"",COUNTIF(G$4:G45,"?*"))</f>
         <v>41</v>
@@ -5406,7 +5539,10 @@
       </c>
     </row>
     <row r="46" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D46" s="8"/>
+      <c r="D46" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G46,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E46" t="str">
         <f>IF(COUNTBLANK(G46)&gt;0,"",COUNTIF(G$4:G46,"?*"))</f>
         <v/>
@@ -5463,7 +5599,10 @@
       </c>
     </row>
     <row r="47" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D47" s="8"/>
+      <c r="D47" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G47,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="20" t="str">
@@ -5512,7 +5651,10 @@
       <c r="U47" s="30"/>
     </row>
     <row r="48" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D48" s="8"/>
+      <c r="D48" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G48,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E48" t="str">
         <f>IF(COUNTBLANK(G48)&gt;0,"",COUNTIF(G$4:G48,"?*"))</f>
         <v/>
@@ -5569,7 +5711,10 @@
       </c>
     </row>
     <row r="49" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D49" s="8"/>
+      <c r="D49" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G49,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E49" t="str">
         <f>IF(COUNTBLANK(G49)&gt;0,"",COUNTIF(G$4:G49,"?*"))</f>
         <v/>
@@ -6046,6 +6191,10 @@
       </c>
     </row>
     <row r="57" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D57" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G57,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E57" t="str">
         <f>IF(COUNTBLANK(G57)&gt;0,"",COUNTIF(G$4:G57,"?*"))</f>
         <v/>
@@ -6102,7 +6251,10 @@
       </c>
     </row>
     <row r="58" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D58" s="8"/>
+      <c r="D58" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G58,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E58" t="str">
         <f>IF(COUNTBLANK(G58)&gt;0,"",COUNTIF(G$4:G58,"?*"))</f>
         <v/>
@@ -6159,7 +6311,10 @@
       </c>
     </row>
     <row r="59" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D59" s="8"/>
+      <c r="D59" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G59,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E59" t="str">
         <f>IF(COUNTBLANK(G59)&gt;0,"",COUNTIF(G$4:G59,"?*"))</f>
         <v/>
@@ -6636,6 +6791,10 @@
       </c>
     </row>
     <row r="67" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D67" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G67,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E67" t="str">
         <f>IF(COUNTBLANK(G67)&gt;0,"",COUNTIF(G$4:G67,"?*"))</f>
         <v/>
@@ -6692,7 +6851,10 @@
       </c>
     </row>
     <row r="68" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D68" s="8"/>
+      <c r="D68" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G68,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E68" t="str">
         <f>IF(COUNTBLANK(G68)&gt;0,"",COUNTIF(G$4:G68,"?*"))</f>
         <v/>
@@ -6749,7 +6911,10 @@
       </c>
     </row>
     <row r="69" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D69" s="8"/>
+      <c r="D69" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G69,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E69" t="str">
         <f>IF(COUNTBLANK(G69)&gt;0,"",COUNTIF(G$4:G69,"?*"))</f>
         <v/>
@@ -6806,7 +6971,10 @@
       </c>
     </row>
     <row r="70" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D70" s="8"/>
+      <c r="D70" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G70,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E70" t="str">
         <f>IF(COUNTBLANK(G70)&gt;0,"",COUNTIF(G$4:G70,"?*"))</f>
         <v/>
@@ -6863,7 +7031,10 @@
       </c>
     </row>
     <row r="71" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D71" s="8"/>
+      <c r="D71" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G71,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E71" t="str">
         <f>IF(COUNTBLANK(G71)&gt;0,"",COUNTIF(G$4:G71,"?*"))</f>
         <v/>
@@ -7340,6 +7511,10 @@
       </c>
     </row>
     <row r="79" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D79" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G79,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E79" t="str">
         <f>IF(COUNTBLANK(G79)&gt;0,"",COUNTIF(G$4:G79,"?*"))</f>
         <v/>
@@ -7396,7 +7571,10 @@
       </c>
     </row>
     <row r="80" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D80" s="8"/>
+      <c r="D80" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G80,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E80" t="str">
         <f>IF(COUNTBLANK(G80)&gt;0,"",COUNTIF(G$4:G80,"?*"))</f>
         <v/>
@@ -7453,7 +7631,10 @@
       </c>
     </row>
     <row r="81" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D81" s="8"/>
+      <c r="D81" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G81,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E81" t="str">
         <f>IF(COUNTBLANK(G81)&gt;0,"",COUNTIF(G$4:G81,"?*"))</f>
         <v/>
@@ -7930,6 +8111,10 @@
       </c>
     </row>
     <row r="89" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D89" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G89,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E89" t="str">
         <f>IF(COUNTBLANK(G89)&gt;0,"",COUNTIF(G$4:G89,"?*"))</f>
         <v/>
@@ -7986,7 +8171,10 @@
       </c>
     </row>
     <row r="90" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D90" s="8"/>
+      <c r="D90" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G90,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E90" t="str">
         <f>IF(COUNTBLANK(G90)&gt;0,"",COUNTIF(G$4:G90,"?*"))</f>
         <v/>
@@ -8043,7 +8231,10 @@
       </c>
     </row>
     <row r="91" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D91" s="8"/>
+      <c r="D91" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G91,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E91" t="str">
         <f>IF(COUNTBLANK(G91)&gt;0,"",COUNTIF(G$4:G91,"?*"))</f>
         <v/>
@@ -8100,7 +8291,10 @@
       </c>
     </row>
     <row r="92" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D92" s="8"/>
+      <c r="D92" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G92,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E92" t="str">
         <f>IF(COUNTBLANK(G92)&gt;0,"",COUNTIF(G$4:G92,"?*"))</f>
         <v/>
@@ -8157,7 +8351,10 @@
       </c>
     </row>
     <row r="93" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D93" s="8"/>
+      <c r="D93" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G93,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E93" t="str">
         <f>IF(COUNTBLANK(G93)&gt;0,"",COUNTIF(G$4:G93,"?*"))</f>
         <v/>
@@ -8634,6 +8831,10 @@
       </c>
     </row>
     <row r="101" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D101" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G101,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E101" t="str">
         <f>IF(COUNTBLANK(G101)&gt;0,"",COUNTIF(G$4:G101,"?*"))</f>
         <v/>
@@ -8690,7 +8891,10 @@
       </c>
     </row>
     <row r="102" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D102" s="8"/>
+      <c r="D102" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G102,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E102" t="str">
         <f>IF(COUNTBLANK(G102)&gt;0,"",COUNTIF(G$4:G102,"?*"))</f>
         <v/>
@@ -8747,7 +8951,10 @@
       </c>
     </row>
     <row r="103" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D103" s="8"/>
+      <c r="D103" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G103,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E103" t="str">
         <f>IF(COUNTBLANK(G103)&gt;0,"",COUNTIF(G$4:G103,"?*"))</f>
         <v/>
@@ -9224,6 +9431,10 @@
       </c>
     </row>
     <row r="111" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D111" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G111,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E111" t="str">
         <f>IF(COUNTBLANK(G111)&gt;0,"",COUNTIF(G$4:G111,"?*"))</f>
         <v/>
@@ -9280,7 +9491,10 @@
       </c>
     </row>
     <row r="112" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D112" s="8"/>
+      <c r="D112" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G112,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E112" t="str">
         <f>IF(COUNTBLANK(G112)&gt;0,"",COUNTIF(G$4:G112,"?*"))</f>
         <v/>
@@ -9337,7 +9551,10 @@
       </c>
     </row>
     <row r="113" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D113" s="8"/>
+      <c r="D113" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G113,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E113" t="str">
         <f>IF(COUNTBLANK(G113)&gt;0,"",COUNTIF(G$4:G113,"?*"))</f>
         <v/>
@@ -9394,7 +9611,10 @@
       </c>
     </row>
     <row r="114" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D114" s="8"/>
+      <c r="D114" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G114,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E114" t="str">
         <f>IF(COUNTBLANK(G114)&gt;0,"",COUNTIF(G$4:G114,"?*"))</f>
         <v/>
@@ -9451,7 +9671,10 @@
       </c>
     </row>
     <row r="115" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D115" s="8"/>
+      <c r="D115" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G115,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E115" t="str">
         <f>IF(COUNTBLANK(G115)&gt;0,"",COUNTIF(G$4:G115,"?*"))</f>
         <v/>
@@ -9928,6 +10151,10 @@
       </c>
     </row>
     <row r="123" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D123" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G123,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E123" t="str">
         <f>IF(COUNTBLANK(G123)&gt;0,"",COUNTIF(G$4:G123,"?*"))</f>
         <v/>
@@ -9984,7 +10211,10 @@
       </c>
     </row>
     <row r="124" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D124" s="8"/>
+      <c r="D124" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G124,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E124" t="str">
         <f>IF(COUNTBLANK(G124)&gt;0,"",COUNTIF(G$4:G124,"?*"))</f>
         <v/>
@@ -10041,7 +10271,10 @@
       </c>
     </row>
     <row r="125" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D125" s="8"/>
+      <c r="D125" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G125,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E125" t="str">
         <f>IF(COUNTBLANK(G125)&gt;0,"",COUNTIF(G$4:G125,"?*"))</f>
         <v/>
@@ -10518,6 +10751,10 @@
       </c>
     </row>
     <row r="133" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D133" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G133,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E133" t="str">
         <f>IF(COUNTBLANK(G133)&gt;0,"",COUNTIF(G$4:G133,"?*"))</f>
         <v/>
@@ -10574,7 +10811,10 @@
       </c>
     </row>
     <row r="134" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D134" s="8"/>
+      <c r="D134" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G134,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E134" t="str">
         <f>IF(COUNTBLANK(G134)&gt;0,"",COUNTIF(G$4:G134,"?*"))</f>
         <v/>
@@ -10631,7 +10871,10 @@
       </c>
     </row>
     <row r="135" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D135" s="8"/>
+      <c r="D135" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G135,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E135" t="str">
         <f>IF(COUNTBLANK(G135)&gt;0,"",COUNTIF(G$4:G135,"?*"))</f>
         <v/>
@@ -10688,7 +10931,10 @@
       </c>
     </row>
     <row r="136" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D136" s="8"/>
+      <c r="D136" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G136,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E136" t="str">
         <f>IF(COUNTBLANK(G136)&gt;0,"",COUNTIF(G$4:G136,"?*"))</f>
         <v/>
@@ -10745,7 +10991,10 @@
       </c>
     </row>
     <row r="137" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D137" s="8"/>
+      <c r="D137" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G137,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E137" t="str">
         <f>IF(COUNTBLANK(G137)&gt;0,"",COUNTIF(G$4:G137,"?*"))</f>
         <v/>
@@ -11222,6 +11471,10 @@
       </c>
     </row>
     <row r="145" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D145" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G145,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E145" t="str">
         <f>IF(COUNTBLANK(G145)&gt;0,"",COUNTIF(G$4:G145,"?*"))</f>
         <v/>
@@ -11278,7 +11531,10 @@
       </c>
     </row>
     <row r="146" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D146" s="8"/>
+      <c r="D146" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G146,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E146" t="str">
         <f>IF(COUNTBLANK(G146)&gt;0,"",COUNTIF(G$4:G146,"?*"))</f>
         <v/>
@@ -11335,7 +11591,10 @@
       </c>
     </row>
     <row r="147" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D147" s="8"/>
+      <c r="D147" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G147,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E147" t="str">
         <f>IF(COUNTBLANK(G147)&gt;0,"",COUNTIF(G$4:G147,"?*"))</f>
         <v/>
@@ -11812,6 +12071,10 @@
       </c>
     </row>
     <row r="155" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D155" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G155,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E155" t="str">
         <f>IF(COUNTBLANK(G155)&gt;0,"",COUNTIF(G$4:G155,"?*"))</f>
         <v/>
@@ -11868,7 +12131,10 @@
       </c>
     </row>
     <row r="156" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D156" s="8"/>
+      <c r="D156" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G156,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E156" t="str">
         <f>IF(COUNTBLANK(G156)&gt;0,"",COUNTIF(G$4:G156,"?*"))</f>
         <v/>
@@ -11925,7 +12191,10 @@
       </c>
     </row>
     <row r="157" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D157" s="8"/>
+      <c r="D157" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G157,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E157" t="str">
         <f>IF(COUNTBLANK(G157)&gt;0,"",COUNTIF(G$4:G157,"?*"))</f>
         <v/>
@@ -11982,7 +12251,10 @@
       </c>
     </row>
     <row r="158" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D158" s="8"/>
+      <c r="D158" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G158,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E158" t="str">
         <f>IF(COUNTBLANK(G158)&gt;0,"",COUNTIF(G$4:G158,"?*"))</f>
         <v/>
@@ -12039,7 +12311,10 @@
       </c>
     </row>
     <row r="159" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D159" s="8"/>
+      <c r="D159" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G159,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E159" t="str">
         <f>IF(COUNTBLANK(G159)&gt;0,"",COUNTIF(G$4:G159,"?*"))</f>
         <v/>
@@ -12516,6 +12791,10 @@
       </c>
     </row>
     <row r="167" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D167" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G167,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E167" t="str">
         <f>IF(COUNTBLANK(G167)&gt;0,"",COUNTIF(G$4:G167,"?*"))</f>
         <v/>
@@ -12572,7 +12851,10 @@
       </c>
     </row>
     <row r="168" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D168" s="8"/>
+      <c r="D168" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G168,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E168" t="str">
         <f>IF(COUNTBLANK(G168)&gt;0,"",COUNTIF(G$4:G168,"?*"))</f>
         <v/>
@@ -12629,7 +12911,10 @@
       </c>
     </row>
     <row r="169" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D169" s="8"/>
+      <c r="D169" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G169,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E169" t="str">
         <f>IF(COUNTBLANK(G169)&gt;0,"",COUNTIF(G$4:G169,"?*"))</f>
         <v/>
@@ -13106,6 +13391,10 @@
       </c>
     </row>
     <row r="177" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D177" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G177,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E177" t="str">
         <f>IF(COUNTBLANK(G177)&gt;0,"",COUNTIF(G$4:G177,"?*"))</f>
         <v/>
@@ -13162,7 +13451,10 @@
       </c>
     </row>
     <row r="178" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D178" s="8"/>
+      <c r="D178" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G178,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E178" t="str">
         <f>IF(COUNTBLANK(G178)&gt;0,"",COUNTIF(G$4:G178,"?*"))</f>
         <v/>
@@ -13219,7 +13511,10 @@
       </c>
     </row>
     <row r="179" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D179" s="8"/>
+      <c r="D179" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G179,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E179" t="str">
         <f>IF(COUNTBLANK(G179)&gt;0,"",COUNTIF(G$4:G179,"?*"))</f>
         <v/>
@@ -13276,7 +13571,10 @@
       </c>
     </row>
     <row r="180" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D180" s="8"/>
+      <c r="D180" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G180,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E180" t="str">
         <f>IF(COUNTBLANK(G180)&gt;0,"",COUNTIF(G$4:G180,"?*"))</f>
         <v/>
@@ -13333,7 +13631,10 @@
       </c>
     </row>
     <row r="181" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D181" s="8"/>
+      <c r="D181" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G181,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E181" t="str">
         <f>IF(COUNTBLANK(G181)&gt;0,"",COUNTIF(G$4:G181,"?*"))</f>
         <v/>
@@ -13810,6 +14111,10 @@
       </c>
     </row>
     <row r="189" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D189" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G189,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E189" t="str">
         <f>IF(COUNTBLANK(G189)&gt;0,"",COUNTIF(G$4:G189,"?*"))</f>
         <v/>
@@ -13866,7 +14171,10 @@
       </c>
     </row>
     <row r="190" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D190" s="8"/>
+      <c r="D190" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G190,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E190" t="str">
         <f>IF(COUNTBLANK(G190)&gt;0,"",COUNTIF(G$4:G190,"?*"))</f>
         <v/>
@@ -13923,7 +14231,10 @@
       </c>
     </row>
     <row r="191" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D191" s="8"/>
+      <c r="D191" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G191,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E191" t="str">
         <f>IF(COUNTBLANK(G191)&gt;0,"",COUNTIF(G$4:G191,"?*"))</f>
         <v/>
@@ -14400,6 +14711,10 @@
       </c>
     </row>
     <row r="199" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D199" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G199,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E199" t="str">
         <f>IF(COUNTBLANK(G199)&gt;0,"",COUNTIF(G$4:G199,"?*"))</f>
         <v/>
@@ -14456,7 +14771,10 @@
       </c>
     </row>
     <row r="200" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D200" s="8"/>
+      <c r="D200" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G200,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E200" t="str">
         <f>IF(COUNTBLANK(G200)&gt;0,"",COUNTIF(G$4:G200,"?*"))</f>
         <v/>
@@ -14513,7 +14831,10 @@
       </c>
     </row>
     <row r="201" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D201" s="8"/>
+      <c r="D201" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G201,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E201" t="str">
         <f>IF(COUNTBLANK(G201)&gt;0,"",COUNTIF(G$4:G201,"?*"))</f>
         <v/>
@@ -14570,7 +14891,10 @@
       </c>
     </row>
     <row r="202" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D202" s="8"/>
+      <c r="D202" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G202,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E202" t="str">
         <f>IF(COUNTBLANK(G202)&gt;0,"",COUNTIF(G$4:G202,"?*"))</f>
         <v/>
@@ -14627,7 +14951,10 @@
       </c>
     </row>
     <row r="203" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D203" s="8"/>
+      <c r="D203" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G203,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E203" t="str">
         <f>IF(COUNTBLANK(G203)&gt;0,"",COUNTIF(G$4:G203,"?*"))</f>
         <v/>
@@ -15104,6 +15431,10 @@
       </c>
     </row>
     <row r="211" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D211" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G211,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E211" t="str">
         <f>IF(COUNTBLANK(G211)&gt;0,"",COUNTIF(G$4:G211,"?*"))</f>
         <v/>
@@ -15160,7 +15491,10 @@
       </c>
     </row>
     <row r="212" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D212" s="8"/>
+      <c r="D212" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G212,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E212" t="str">
         <f>IF(COUNTBLANK(G212)&gt;0,"",COUNTIF(G$4:G212,"?*"))</f>
         <v/>
@@ -15217,7 +15551,10 @@
       </c>
     </row>
     <row r="213" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D213" s="8"/>
+      <c r="D213" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G213,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E213" t="str">
         <f>IF(COUNTBLANK(G213)&gt;0,"",COUNTIF(G$4:G213,"?*"))</f>
         <v/>
@@ -15694,6 +16031,10 @@
       </c>
     </row>
     <row r="221" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D221" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G221,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E221" t="str">
         <f>IF(COUNTBLANK(G221)&gt;0,"",COUNTIF(G$4:G221,"?*"))</f>
         <v/>
@@ -15750,7 +16091,10 @@
       </c>
     </row>
     <row r="222" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D222" s="8"/>
+      <c r="D222" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G222,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E222" t="str">
         <f>IF(COUNTBLANK(G222)&gt;0,"",COUNTIF(G$4:G222,"?*"))</f>
         <v/>
@@ -15807,7 +16151,10 @@
       </c>
     </row>
     <row r="223" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D223" s="8"/>
+      <c r="D223" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G223,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E223" t="str">
         <f>IF(COUNTBLANK(G223)&gt;0,"",COUNTIF(G$4:G223,"?*"))</f>
         <v/>
@@ -15864,7 +16211,10 @@
       </c>
     </row>
     <row r="224" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D224" s="8"/>
+      <c r="D224" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G224,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E224" t="str">
         <f>IF(COUNTBLANK(G224)&gt;0,"",COUNTIF(G$4:G224,"?*"))</f>
         <v/>
@@ -15921,7 +16271,10 @@
       </c>
     </row>
     <row r="225" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D225" s="8"/>
+      <c r="D225" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G225,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E225" t="str">
         <f>IF(COUNTBLANK(G225)&gt;0,"",COUNTIF(G$4:G225,"?*"))</f>
         <v/>
@@ -16398,6 +16751,10 @@
       </c>
     </row>
     <row r="233" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D233" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G233,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E233" t="str">
         <f>IF(COUNTBLANK(G233)&gt;0,"",COUNTIF(G$4:G233,"?*"))</f>
         <v/>
@@ -16454,7 +16811,10 @@
       </c>
     </row>
     <row r="234" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D234" s="8"/>
+      <c r="D234" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G234,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E234" t="str">
         <f>IF(COUNTBLANK(G234)&gt;0,"",COUNTIF(G$4:G234,"?*"))</f>
         <v/>
@@ -16511,7 +16871,10 @@
       </c>
     </row>
     <row r="235" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D235" s="8"/>
+      <c r="D235" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G235,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E235" t="str">
         <f>IF(COUNTBLANK(G235)&gt;0,"",COUNTIF(G$4:G235,"?*"))</f>
         <v/>
@@ -16988,6 +17351,10 @@
       </c>
     </row>
     <row r="243" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D243" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G243,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E243" t="str">
         <f>IF(COUNTBLANK(G243)&gt;0,"",COUNTIF(G$4:G243,"?*"))</f>
         <v/>
@@ -17044,7 +17411,10 @@
       </c>
     </row>
     <row r="244" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D244" s="8"/>
+      <c r="D244" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G244,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E244" t="str">
         <f>IF(COUNTBLANK(G244)&gt;0,"",COUNTIF(G$4:G244,"?*"))</f>
         <v/>
@@ -17101,7 +17471,10 @@
       </c>
     </row>
     <row r="245" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D245" s="8"/>
+      <c r="D245" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G245,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E245" t="str">
         <f>IF(COUNTBLANK(G245)&gt;0,"",COUNTIF(G$4:G245,"?*"))</f>
         <v/>
@@ -17158,7 +17531,10 @@
       </c>
     </row>
     <row r="246" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D246" s="8"/>
+      <c r="D246" s="8" t="str">
+        <f>IF(LEN(_xlfn.IFNA(VLOOKUP(G246,EnElServer!A:A,1,FALSE),""))&gt;0,"x","")</f>
+        <v/>
+      </c>
       <c r="E246" t="str">
         <f>IF(COUNTBLANK(G246)&gt;0,"",COUNTIF(G$4:G246,"?*"))</f>
         <v/>
@@ -17227,7 +17603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
@@ -17683,7 +18059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C7C90C-DC2C-49DB-BA75-D5F1F405505C}">
   <dimension ref="A1:B383"/>
   <sheetViews>
-    <sheetView topLeftCell="A378" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A384" sqref="A384"/>
     </sheetView>
   </sheetViews>
@@ -20441,7 +20817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77182073-2D58-4EA1-9D23-0ED8915BBAB3}">
   <dimension ref="A1:D174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -22164,4 +22540,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA93F7D-9A21-43F8-BA27-E55A63CE0E72}">
+  <dimension ref="A1:A42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
+        <v>638</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>